<commit_message>
add XS and XQ to controls
</commit_message>
<xml_diff>
--- a/data/controls/metadata.xlsx
+++ b/data/controls/metadata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="118">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -527,6 +527,72 @@
       </rPr>
       <t>Omicron/BA.2/21L</t>
     </r>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>OM981060.1</t>
+  </si>
+  <si>
+    <t>USA/OH-CDC-MMB14658183/2022</t>
+  </si>
+  <si>
+    <t>2022-03-07</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>USA/CO-CDC-FG-248528/2022</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10998663</t>
+  </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
+  <si>
+    <t>EPI_ISL_9425763</t>
+  </si>
+  <si>
+    <t>XQ</t>
+  </si>
+  <si>
+    <t>OW142543.1</t>
+  </si>
+  <si>
+    <t>England/MILK-38AA91B/2022</t>
+  </si>
+  <si>
+    <t>2022-02-28</t>
+  </si>
+  <si>
+    <t>England/LSPA-3943EF6/2022</t>
+  </si>
+  <si>
+    <t>2022-03-05</t>
+  </si>
+  <si>
+    <t>OW192527.1</t>
+  </si>
+  <si>
+    <t>OM477123.1</t>
+  </si>
+  <si>
+    <t>468</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10976407</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10725431</t>
+  </si>
+  <si>
+    <t>4322:5385</t>
+  </si>
+  <si>
+    <t>9055:10447</t>
   </si>
 </sst>
 </file>
@@ -605,7 +671,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -672,12 +738,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -746,6 +874,32 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1054,16 +1208,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="4" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
@@ -1601,6 +1755,138 @@
         <v>49</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add XS breakpoints to metadata
</commit_message>
<xml_diff>
--- a/data/controls/metadata.xlsx
+++ b/data/controls/metadata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="119">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -592,7 +592,44 @@
     <t>4322:5385</t>
   </si>
   <si>
-    <t>9055:10447</t>
+    <t>9056:10448</t>
+  </si>
+  <si>
+    <r>
+      <t>210:10029|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,10449:29742|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1210,8 +1247,8 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,7 +1808,9 @@
       <c r="E16" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="G16" s="33" t="s">
         <v>117</v>
       </c>
@@ -1804,7 +1843,9 @@
       <c r="E17" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="38"/>
+      <c r="F17" s="38" t="s">
+        <v>118</v>
+      </c>
       <c r="G17" s="38" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
add XD to controls
</commit_message>
<xml_diff>
--- a/data/controls/metadata.xlsx
+++ b/data/controls/metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14748" windowHeight="6168"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9984"/>
   </bookViews>
   <sheets>
     <sheet name="github" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -629,6 +629,131 @@
         <scheme val="minor"/>
       </rPr>
       <t>Omicron/BA.1/21K</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>241:4321|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,5386:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>OM990739.1</t>
+  </si>
+  <si>
+    <t>FRA/IHUMI-6070VR/2022</t>
+  </si>
+  <si>
+    <t>OM990851.1</t>
+  </si>
+  <si>
+    <t>FRA/IHUCOVID-64762/2022</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>2022-02-09</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>21988:22672,25470:25583</t>
+  </si>
+  <si>
+    <r>
+      <t>210:21987|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,22673:25469|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,25584:29742|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta/21J</t>
     </r>
   </si>
 </sst>
@@ -708,7 +833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -775,74 +900,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -913,30 +976,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1245,10 +1297,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1310,7 @@
     <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="55.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" style="4" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
@@ -1303,245 +1355,245 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="A2" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>65</v>
+      <c r="I2" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J4" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K5" s="27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K7" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>50</v>
@@ -1549,270 +1601,270 @@
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="24" t="s">
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>63</v>
+      <c r="J10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="25" t="s">
+      <c r="A11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E12" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F12" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G12" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="I12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="24" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K15" s="24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>117</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>23</v>
@@ -1820,34 +1872,34 @@
       <c r="I16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="K16" s="34" t="s">
-        <v>96</v>
+      <c r="J16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>117</v>
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>23</v>
@@ -1855,76 +1907,150 @@
       <c r="I17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="K17" s="39" t="s">
-        <v>96</v>
+      <c r="J17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
-        <v>107</v>
+      <c r="A18" s="31" t="s">
+        <v>98</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="K18" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B21" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E21" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38" t="s">
+      <c r="F21" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H21" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I21" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="38" t="s">
+      <c r="J21" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K21" s="33" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add XM to controls
</commit_message>
<xml_diff>
--- a/data/controls/metadata.xlsx
+++ b/data/controls/metadata.xlsx
@@ -15,11 +15,12 @@
     <sheet name="github" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -754,6 +755,70 @@
         <scheme val="minor"/>
       </rPr>
       <t>Delta/21J</t>
+    </r>
+  </si>
+  <si>
+    <t>XM</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t>ON199453.1</t>
+  </si>
+  <si>
+    <t>OW090848.1</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10536094</t>
+  </si>
+  <si>
+    <t>England/MILK-3796834/2022</t>
+  </si>
+  <si>
+    <t>EPI_ISL_11903369</t>
+  </si>
+  <si>
+    <t>USA/NY-Broad-CRSP_WH5TJZ42BYV4BC3T/2022</t>
+  </si>
+  <si>
+    <t>2022-03-28</t>
+  </si>
+  <si>
+    <t>18164:19954</t>
+  </si>
+  <si>
+    <r>
+      <t>241:18163|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,19955:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
     </r>
   </si>
 </sst>
@@ -905,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -989,6 +1054,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1297,10 +1365,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,143 +1982,213 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="19" t="s">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="K19" s="33" t="s">
-        <v>96</v>
+      <c r="J18" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="31" t="s">
-        <v>10</v>
+        <v>117</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B23" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C23" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E23" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F23" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G23" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H23" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I23" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J23" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="33" t="s">
+      <c r="K23" s="33" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update controls breakpoints and add col sc2rf_lineage
</commit_message>
<xml_diff>
--- a/data/controls/metadata.xlsx
+++ b/data/controls/metadata.xlsx
@@ -9,18 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9984"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544"/>
   </bookViews>
   <sheets>
     <sheet name="github" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="141">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -175,8 +174,17 @@
     <t>XF</t>
   </si>
   <si>
-    <r>
-      <t>210:18893|</t>
+    <t>breakpoints</t>
+  </si>
+  <si>
+    <t>clades_regions</t>
+  </si>
+  <si>
+    <t>15241:15713</t>
+  </si>
+  <si>
+    <r>
+      <t>210:21618|</t>
     </r>
     <r>
       <rPr>
@@ -195,7 +203,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>,19220:29742|</t>
+      <t>,21762:29742|</t>
     </r>
     <r>
       <rPr>
@@ -209,8 +217,194 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>241:15240|</t>
+    <t>21619:21761</t>
+  </si>
+  <si>
+    <t>XH</t>
+  </si>
+  <si>
+    <t>448</t>
+  </si>
+  <si>
+    <t>XG</t>
+  </si>
+  <si>
+    <t>447</t>
+  </si>
+  <si>
+    <t>XE</t>
+  </si>
+  <si>
+    <t>454</t>
+  </si>
+  <si>
+    <t>England/MILK-3795589/2022</t>
+  </si>
+  <si>
+    <t>OW091023.1</t>
+  </si>
+  <si>
+    <t>OW084783.1</t>
+  </si>
+  <si>
+    <t>Scotland/QEUH-37E04A0/2022</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>England/MILK-3729AD6/2022</t>
+  </si>
+  <si>
+    <t>OW016842.1</t>
+  </si>
+  <si>
+    <t>2022-02-16</t>
+  </si>
+  <si>
+    <t>England/BRBR-3899D04/2022</t>
+  </si>
+  <si>
+    <t>OW137497.1</t>
+  </si>
+  <si>
+    <t>2022-02-27</t>
+  </si>
+  <si>
+    <t>England/MILK-37D141B/2022</t>
+  </si>
+  <si>
+    <t>OW042525.1</t>
+  </si>
+  <si>
+    <t>2022-02-20</t>
+  </si>
+  <si>
+    <t>England/MILK-385C31A/2022</t>
+  </si>
+  <si>
+    <t>OW126705.1</t>
+  </si>
+  <si>
+    <t>2022-02-24</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10245373</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10709177</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10417914</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10641208</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10535975</t>
+  </si>
+  <si>
+    <t>2022-02-19</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10532208</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>OM981060.1</t>
+  </si>
+  <si>
+    <t>USA/OH-CDC-MMB14658183/2022</t>
+  </si>
+  <si>
+    <t>2022-03-07</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>USA/CO-CDC-FG-248528/2022</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10998663</t>
+  </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
+  <si>
+    <t>EPI_ISL_9425763</t>
+  </si>
+  <si>
+    <t>XQ</t>
+  </si>
+  <si>
+    <t>OW142543.1</t>
+  </si>
+  <si>
+    <t>England/MILK-38AA91B/2022</t>
+  </si>
+  <si>
+    <t>2022-02-28</t>
+  </si>
+  <si>
+    <t>England/LSPA-3943EF6/2022</t>
+  </si>
+  <si>
+    <t>2022-03-05</t>
+  </si>
+  <si>
+    <t>OW192527.1</t>
+  </si>
+  <si>
+    <t>OM477123.1</t>
+  </si>
+  <si>
+    <t>468</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10976407</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10725431</t>
+  </si>
+  <si>
+    <t>4322:5385</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>OM990739.1</t>
+  </si>
+  <si>
+    <t>FRA/IHUMI-6070VR/2022</t>
+  </si>
+  <si>
+    <t>OM990851.1</t>
+  </si>
+  <si>
+    <t>FRA/IHUCOVID-64762/2022</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>2022-02-09</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>21988:22672,25470:25583</t>
+  </si>
+  <si>
+    <r>
+      <t>210:21987|</t>
     </r>
     <r>
       <rPr>
@@ -219,16 +413,243 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,22673:25469|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>Omicron/BA.1/21K</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,25584:29742|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+  </si>
+  <si>
+    <t>XM</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t>ON199453.1</t>
+  </si>
+  <si>
+    <t>OW090848.1</t>
+  </si>
+  <si>
+    <t>EPI_ISL_10536094</t>
+  </si>
+  <si>
+    <t>England/MILK-3796834/2022</t>
+  </si>
+  <si>
+    <t>EPI_ISL_11903369</t>
+  </si>
+  <si>
+    <t>USA/NY-Broad-CRSP_WH5TJZ42BYV4BC3T/2022</t>
+  </si>
+  <si>
+    <t>2022-03-28</t>
+  </si>
+  <si>
+    <r>
+      <t>670:10447|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,11537:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <t>10448:11536</t>
+  </si>
+  <si>
+    <r>
+      <t>174:21618|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>,21762:29742|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>670:5386|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,8393:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>670:10447|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,11537:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>670:15240|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>,15714:29510|</t>
     </r>
     <r>
@@ -243,20 +664,8 @@
     </r>
   </si>
   <si>
-    <t>breakpoints</t>
-  </si>
-  <si>
-    <t>clades_regions</t>
-  </si>
-  <si>
-    <t>15241:15713</t>
-  </si>
-  <si>
-    <t>18894:19219</t>
-  </si>
-  <si>
-    <r>
-      <t>210:21762|</t>
+    <r>
+      <t>670:17410|</t>
     </r>
     <r>
       <rPr>
@@ -266,11 +675,128 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,19955:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <t>17411:19954</t>
+  </si>
+  <si>
+    <r>
+      <t>210:9053|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Delta/21J</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,10449:29742|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+  </si>
+  <si>
+    <t>9054:10448</t>
+  </si>
+  <si>
+    <r>
+      <t>670:4321|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.1/21K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,5386:29510|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omicron/BA.2/21L</t>
+    </r>
+  </si>
+  <si>
+    <t>5387:8382</t>
+  </si>
+  <si>
+    <r>
+      <t>210:21987|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Delta/21J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -289,537 +815,7 @@
     </r>
   </si>
   <si>
-    <t>21763:22577</t>
-  </si>
-  <si>
-    <r>
-      <t>210:21618|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Delta/21J</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,21762:29742|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-  </si>
-  <si>
-    <t>21619:21761</t>
-  </si>
-  <si>
-    <t>XH</t>
-  </si>
-  <si>
-    <t>448</t>
-  </si>
-  <si>
-    <t>XG</t>
-  </si>
-  <si>
-    <t>447</t>
-  </si>
-  <si>
-    <t>XE</t>
-  </si>
-  <si>
-    <t>454</t>
-  </si>
-  <si>
-    <t>England/MILK-3795589/2022</t>
-  </si>
-  <si>
-    <t>OW091023.1</t>
-  </si>
-  <si>
-    <t>OW084783.1</t>
-  </si>
-  <si>
-    <t>Scotland/QEUH-37E04A0/2022</t>
-  </si>
-  <si>
-    <t>Scotland</t>
-  </si>
-  <si>
-    <t>England/MILK-3729AD6/2022</t>
-  </si>
-  <si>
-    <t>OW016842.1</t>
-  </si>
-  <si>
-    <t>2022-02-16</t>
-  </si>
-  <si>
-    <t>England/BRBR-3899D04/2022</t>
-  </si>
-  <si>
-    <t>OW137497.1</t>
-  </si>
-  <si>
-    <t>2022-02-27</t>
-  </si>
-  <si>
-    <t>England/MILK-37D141B/2022</t>
-  </si>
-  <si>
-    <t>OW042525.1</t>
-  </si>
-  <si>
-    <t>2022-02-20</t>
-  </si>
-  <si>
-    <t>England/MILK-385C31A/2022</t>
-  </si>
-  <si>
-    <t>OW126705.1</t>
-  </si>
-  <si>
-    <t>2022-02-24</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10245373</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10709177</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10417914</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10641208</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10535975</t>
-  </si>
-  <si>
-    <t>2022-02-19</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10532208</t>
-  </si>
-  <si>
-    <r>
-      <t>241:10449|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,11537:29510|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.2/21L</t>
-    </r>
-  </si>
-  <si>
-    <t>10450:11536</t>
-  </si>
-  <si>
-    <r>
-      <t>241:5386|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,8393:29510|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.2/21L</t>
-    </r>
-  </si>
-  <si>
-    <t>5367:8382</t>
-  </si>
-  <si>
-    <r>
-      <t>241:10449|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,11537:29510|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.2/21L</t>
-    </r>
-  </si>
-  <si>
-    <t>XS</t>
-  </si>
-  <si>
-    <t>OM981060.1</t>
-  </si>
-  <si>
-    <t>USA/OH-CDC-MMB14658183/2022</t>
-  </si>
-  <si>
-    <t>2022-03-07</t>
-  </si>
-  <si>
-    <t>471</t>
-  </si>
-  <si>
-    <t>USA/CO-CDC-FG-248528/2022</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10998663</t>
-  </si>
-  <si>
-    <t>2022-01-19</t>
-  </si>
-  <si>
-    <t>EPI_ISL_9425763</t>
-  </si>
-  <si>
-    <t>XQ</t>
-  </si>
-  <si>
-    <t>OW142543.1</t>
-  </si>
-  <si>
-    <t>England/MILK-38AA91B/2022</t>
-  </si>
-  <si>
-    <t>2022-02-28</t>
-  </si>
-  <si>
-    <t>England/LSPA-3943EF6/2022</t>
-  </si>
-  <si>
-    <t>2022-03-05</t>
-  </si>
-  <si>
-    <t>OW192527.1</t>
-  </si>
-  <si>
-    <t>OM477123.1</t>
-  </si>
-  <si>
-    <t>468</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10976407</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10725431</t>
-  </si>
-  <si>
-    <t>4322:5385</t>
-  </si>
-  <si>
-    <t>9056:10448</t>
-  </si>
-  <si>
-    <r>
-      <t>210:10029|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delta/21J</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,10449:29742|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>241:4321|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,5386:29510|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.2/21L</t>
-    </r>
-  </si>
-  <si>
-    <t>XD</t>
-  </si>
-  <si>
-    <t>444</t>
-  </si>
-  <si>
-    <t>OM990739.1</t>
-  </si>
-  <si>
-    <t>FRA/IHUMI-6070VR/2022</t>
-  </si>
-  <si>
-    <t>OM990851.1</t>
-  </si>
-  <si>
-    <t>FRA/IHUCOVID-64762/2022</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>2022-02-09</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>21988:22672,25470:25583</t>
-  </si>
-  <si>
-    <r>
-      <t>210:21987|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delta/21J</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,22673:25469|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,25584:29742|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delta/21J</t>
-    </r>
-  </si>
-  <si>
-    <t>XM</t>
-  </si>
-  <si>
-    <t>472</t>
-  </si>
-  <si>
-    <t>ON199453.1</t>
-  </si>
-  <si>
-    <t>OW090848.1</t>
-  </si>
-  <si>
-    <t>EPI_ISL_10536094</t>
-  </si>
-  <si>
-    <t>England/MILK-3796834/2022</t>
-  </si>
-  <si>
-    <t>EPI_ISL_11903369</t>
-  </si>
-  <si>
-    <t>USA/NY-Broad-CRSP_WH5TJZ42BYV4BC3T/2022</t>
-  </si>
-  <si>
-    <t>2022-03-28</t>
-  </si>
-  <si>
-    <t>18164:19954</t>
-  </si>
-  <si>
-    <r>
-      <t>241:18163|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.1/21K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,19955:29510|</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Omicron/BA.2/21L</t>
-    </r>
+    <t>21988:22577</t>
   </si>
 </sst>
 </file>
@@ -898,7 +894,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -965,12 +961,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1057,6 +1093,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1367,7 +1415,7 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1379,7 +1427,7 @@
     <col min="4" max="4" width="13.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="76.109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="37.109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" style="4" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="5" customWidth="1"/>
@@ -1404,10 +1452,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>4</v>
@@ -1424,95 +1472,95 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>92</v>
+        <v>127</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>128</v>
       </c>
       <c r="H4" s="31" t="s">
         <v>9</v>
@@ -1521,33 +1569,33 @@
         <v>10</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>92</v>
+        <v>60</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>128</v>
       </c>
       <c r="H5" s="27" t="s">
         <v>9</v>
@@ -1556,10 +1604,10 @@
         <v>10</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1578,11 +1626,11 @@
       <c r="E6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>51</v>
+      <c r="F6" s="35" t="s">
+        <v>129</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>9</v>
@@ -1614,10 +1662,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>9</v>
@@ -1649,10 +1697,10 @@
         <v>21</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>23</v>
@@ -1684,10 +1732,10 @@
         <v>21</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>23</v>
@@ -1719,10 +1767,10 @@
         <v>30</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>9</v>
@@ -1754,10 +1802,10 @@
         <v>30</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>9</v>
@@ -1774,25 +1822,25 @@
     </row>
     <row r="12" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>9</v>
@@ -1801,68 +1849,68 @@
         <v>10</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J13" s="26" t="s">
         <v>41</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>9</v>
@@ -1871,33 +1919,33 @@
         <v>10</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>9</v>
@@ -1906,10 +1954,10 @@
         <v>10</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1929,10 +1977,10 @@
         <v>45</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>23</v>
@@ -1964,10 +2012,10 @@
         <v>45</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>23</v>
@@ -1984,25 +2032,25 @@
     </row>
     <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>141</v>
-      </c>
       <c r="G18" s="26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>23</v>
@@ -2011,33 +2059,33 @@
         <v>24</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C19" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>140</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>9</v>
@@ -2046,33 +2094,33 @@
         <v>10</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>23</v>
@@ -2081,33 +2129,33 @@
         <v>24</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>23</v>
@@ -2116,33 +2164,33 @@
         <v>24</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H22" s="31" t="s">
         <v>9</v>
@@ -2151,33 +2199,33 @@
         <v>10</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C23" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="34" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>116</v>
       </c>
       <c r="H23" s="33" t="s">
         <v>9</v>
@@ -2186,10 +2234,10 @@
         <v>10</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>